<commit_message>
Larger restructuring of the Predicer. This code includes the structure, upon which Predicer is to be built.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D0A8C-29C1-45BF-BB08-982C5F5C12C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBCA8BA-398E-40A8-A677-1B154A4F0629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="commodities" sheetId="9" r:id="rId1"/>
+    <sheet name="resources" sheetId="9" r:id="rId1"/>
     <sheet name="node_def" sheetId="1" r:id="rId2"/>
-    <sheet name="unit_def" sheetId="2" r:id="rId3"/>
+    <sheet name="process_def" sheetId="2" r:id="rId3"/>
     <sheet name="flow" sheetId="5" r:id="rId4"/>
     <sheet name="prices" sheetId="6" r:id="rId5"/>
-    <sheet name="transfer" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
-  <si>
-    <t>commodity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>dh</t>
   </si>
@@ -52,9 +48,6 @@
     <t>wind</t>
   </si>
   <si>
-    <t>balance</t>
-  </si>
-  <si>
     <t>gas</t>
   </si>
   <si>
@@ -64,9 +57,6 @@
     <t>bio</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
     <t>eff</t>
   </si>
   <si>
@@ -88,24 +78,6 @@
     <t>unit_bio1</t>
   </si>
   <si>
-    <t>node_from</t>
-  </si>
-  <si>
-    <t>node_to</t>
-  </si>
-  <si>
-    <t>cap_from</t>
-  </si>
-  <si>
-    <t>cap_to</t>
-  </si>
-  <si>
-    <t>losses</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
     <t>input_node</t>
   </si>
   <si>
@@ -124,15 +96,6 @@
     <t>unit_gt2</t>
   </si>
   <si>
-    <t>transfer</t>
-  </si>
-  <si>
-    <t>node_dh1__to__node_dh2</t>
-  </si>
-  <si>
-    <t>node_elec1__to__node_elec2</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -160,9 +123,6 @@
     <t>VOM_cost</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>min_load</t>
   </si>
   <si>
@@ -184,10 +144,52 @@
     <t>unit_windturb1</t>
   </si>
   <si>
-    <t>wind_availableB</t>
-  </si>
-  <si>
     <t>windB</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>is_commodity</t>
+  </si>
+  <si>
+    <t>has_balance</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>transfer_dhA_dhB</t>
+  </si>
+  <si>
+    <t>transfer_dhB_dhB</t>
+  </si>
+  <si>
+    <t>transfer_elecA_elecB</t>
+  </si>
+  <si>
+    <t>transfer_elecB_elecA</t>
+  </si>
+  <si>
+    <t>ramp_up</t>
+  </si>
+  <si>
+    <t>ramp_down</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>unit_CHP1_dh</t>
+  </si>
+  <si>
+    <t>unit_CHP1_elec</t>
+  </si>
+  <si>
+    <t>is_CF</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -515,47 +517,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF99E4D-86B0-48F4-832E-8948932567B4}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,115 +602,129 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -697,261 +734,553 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B317E83-B82C-4F97-9016-F4FF07D7D9BF}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.2</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.2</v>
+      </c>
+      <c r="L4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0.4</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0.2</v>
+      </c>
+      <c r="L7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+      <c r="L8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.4</v>
+      </c>
+      <c r="H9">
+        <v>0.3</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9">
+        <v>0.3</v>
+      </c>
+      <c r="L9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.4</v>
+      </c>
+      <c r="H10">
+        <v>0.3</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.1</v>
+      </c>
+      <c r="L10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>0.2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11">
+        <v>0.3</v>
+      </c>
+      <c r="L11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>48</v>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.99</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0.5</v>
+      </c>
+      <c r="L12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.99</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.4</v>
+      </c>
+      <c r="L13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.99</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0.4</v>
+      </c>
+      <c r="L14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.99</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0.5</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -961,140 +1290,133 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD40D804-01EB-47A4-AE91-C7D0229E2D4B}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4">
+        <v>43831</v>
+      </c>
       <c r="C1" s="4">
-        <v>43831</v>
+        <v>43832</v>
       </c>
       <c r="D1" s="4">
-        <v>43832</v>
+        <v>43833</v>
       </c>
       <c r="E1" s="4">
-        <v>43833</v>
+        <v>43834</v>
       </c>
       <c r="F1" s="4">
-        <v>43834</v>
+        <v>43835</v>
       </c>
       <c r="G1" s="4">
-        <v>43835</v>
+        <v>43836</v>
       </c>
       <c r="H1" s="4">
-        <v>43836</v>
+        <v>43837</v>
       </c>
       <c r="I1" s="4">
-        <v>43837</v>
+        <v>43838</v>
       </c>
       <c r="J1" s="4">
-        <v>43838</v>
+        <v>43839</v>
       </c>
       <c r="K1" s="4">
-        <v>43839</v>
-      </c>
-      <c r="L1" s="4">
         <v>43840</v>
       </c>
+      <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>-1.8</v>
       </c>
       <c r="C2" s="3">
-        <v>-1.8</v>
+        <v>-3.5</v>
       </c>
       <c r="D2" s="3">
+        <v>-6.6</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-12.7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-12.8</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-10</v>
+      </c>
+      <c r="H2" s="3">
+        <v>-7.7</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-7.6</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-2.5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>-3.7</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-3.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-4.2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-7.1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-11.1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>-6.4</v>
+      </c>
+      <c r="H3" s="3">
+        <v>-3.3</v>
+      </c>
+      <c r="I3" s="3">
         <v>-3.5</v>
       </c>
-      <c r="E2" s="3">
-        <v>-6.6</v>
-      </c>
-      <c r="F2" s="3">
-        <v>-12.7</v>
-      </c>
-      <c r="G2" s="3">
-        <v>-12.8</v>
-      </c>
-      <c r="H2" s="3">
-        <v>-10</v>
-      </c>
-      <c r="I2" s="3">
-        <v>-7.7</v>
-      </c>
-      <c r="J2" s="3">
-        <v>-7.6</v>
-      </c>
-      <c r="K2" s="3">
-        <v>-2.5</v>
-      </c>
-      <c r="L2" s="3">
-        <v>-3.7</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-3.6</v>
-      </c>
-      <c r="E3" s="3">
-        <v>-4.2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-7.1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>-11.1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>-6.4</v>
-      </c>
-      <c r="I3" s="3">
-        <v>-3.3</v>
-      </c>
       <c r="J3" s="3">
-        <v>-3.5</v>
+        <v>-2.1</v>
       </c>
       <c r="K3" s="3">
-        <v>-2.1</v>
-      </c>
-      <c r="L3" s="3">
         <v>-2.2000000000000002</v>
       </c>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-2</v>
       </c>
       <c r="C4" s="3">
         <v>-2</v>
@@ -1123,94 +1445,86 @@
       <c r="K4" s="3">
         <v>-2</v>
       </c>
-      <c r="L4" s="3">
-        <v>-2</v>
-      </c>
+      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-1.1000000000000001</v>
       </c>
       <c r="C5" s="3">
+        <v>-1.2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.9</v>
+      </c>
+      <c r="E5" s="3">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
+        <v>-0.8</v>
+      </c>
+      <c r="G5" s="3">
         <v>-1.2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>-0.9</v>
-      </c>
-      <c r="F5" s="3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="G5" s="3">
-        <v>-0.8</v>
       </c>
       <c r="H5" s="3">
         <v>-1.2</v>
       </c>
       <c r="I5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>-0.8</v>
+      </c>
+      <c r="K5" s="3">
         <v>-1.2</v>
       </c>
-      <c r="J5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>-0.8</v>
-      </c>
-      <c r="L5" s="3">
-        <v>-1.2</v>
-      </c>
+      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C6" s="3">
-        <v>4.5</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="3">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="E6" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="F6" s="3">
-        <v>3.1</v>
+        <v>1.7</v>
       </c>
       <c r="G6" s="3">
-        <v>3.4</v>
+        <v>1.3</v>
       </c>
       <c r="H6" s="3">
-        <v>3.9</v>
+        <v>0.7</v>
       </c>
       <c r="I6" s="3">
-        <v>4.8</v>
+        <v>0.6</v>
       </c>
       <c r="J6" s="3">
-        <v>4.8</v>
+        <v>0.7</v>
       </c>
       <c r="K6" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="L6" s="3">
-        <v>3.9</v>
-      </c>
+        <v>0.7</v>
+      </c>
+      <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7"/>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1220,12 +1534,11 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1238,7 +1551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71A3C8B-32E4-43A2-86A7-9D0D83F1C332}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1276,7 +1591,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1311,7 +1626,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1346,7 +1661,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1381,7 +1696,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1416,7 +1731,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1451,7 +1766,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1488,96 +1803,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF7DCD5-37F1-4A06-946A-7D41EC709552}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added functions for building constraints, as well as fixed some issues.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB93A265-2292-40C4-9120-0885AC5F33E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FF20ED-79B0-4E4A-990B-F58D1B33B255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="5" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>node</t>
   </si>
@@ -318,6 +318,21 @@
   </si>
   <si>
     <t>res_down</t>
+  </si>
+  <si>
+    <t>pv2</t>
+  </si>
+  <si>
+    <t>pv2,s1</t>
+  </si>
+  <si>
+    <t>pv2,s2</t>
+  </si>
+  <si>
+    <t>pv2,s3</t>
+  </si>
+  <si>
+    <t>is_cf_fix</t>
   </si>
 </sst>
 </file>
@@ -697,7 +712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2527,26 +2544,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -2554,34 +2572,37 @@
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2589,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
@@ -2598,25 +2619,28 @@
         <v>1</v>
       </c>
       <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
         <v>0.9</v>
       </c>
-      <c r="G2" s="8">
+      <c r="H2" s="8">
         <v>0.3</v>
       </c>
-      <c r="H2" s="8">
-        <v>1</v>
-      </c>
       <c r="I2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
         <v>4</v>
       </c>
-      <c r="K2" s="8">
+      <c r="L2" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2627,22 +2651,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
       </c>
       <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
         <v>3</v>
       </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
       <c r="H3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="8">
         <v>0</v>
@@ -2650,8 +2674,11 @@
       <c r="K3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2662,22 +2689,22 @@
         <v>0</v>
       </c>
       <c r="D4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
         <v>0.7</v>
       </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
       <c r="H4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="8">
         <v>0</v>
@@ -2685,8 +2712,11 @@
       <c r="K4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2694,25 +2724,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
       </c>
       <c r="E5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8">
         <v>1</v>
       </c>
       <c r="G5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="8">
         <v>0</v>
@@ -2720,74 +2750,121 @@
       <c r="K5" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G7" s="8">
         <v>0.99</v>
       </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
         <v>3</v>
       </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2897,10 +2974,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,22 +3229,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
       </c>
       <c r="E10" s="6">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F10" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="6">
         <v>1</v>
@@ -3181,10 +3258,10 @@
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -3204,19 +3281,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
@@ -3233,24 +3310,50 @@
         <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3301,15 +3404,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A4637A-7829-48D6-AE54-2E654AB1A427}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -3322,8 +3425,17 @@
       <c r="D1" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3338,9 +3450,19 @@
         <f>1*B2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>1*E2</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>1*E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3355,9 +3477,19 @@
         <f t="shared" ref="D3:D25" si="1">1*B3</f>
         <v>0.4</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0.4</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F25" si="2">1*E3</f>
+        <v>0.4</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G25" si="3">1*E3</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -3372,9 +3504,19 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.125</v>
       </c>
@@ -3389,9 +3531,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.16666666666666699</v>
       </c>
@@ -3406,9 +3558,19 @@
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.20833333333333301</v>
       </c>
@@ -3423,9 +3585,19 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.25</v>
       </c>
@@ -3440,9 +3612,19 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.29166666666666702</v>
       </c>
@@ -3457,9 +3639,19 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.33333333333333298</v>
       </c>
@@ -3474,9 +3666,19 @@
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0.4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.375</v>
       </c>
@@ -3491,9 +3693,19 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -3508,9 +3720,19 @@
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>0.7</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -3525,9 +3747,19 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.5</v>
       </c>
@@ -3542,9 +3774,19 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -3559,9 +3801,19 @@
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>0.8</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.58333333333333304</v>
       </c>
@@ -3576,9 +3828,19 @@
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>0.9</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.625</v>
       </c>
@@ -3593,9 +3855,19 @@
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>0.2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.66666666666666696</v>
       </c>
@@ -3610,9 +3882,19 @@
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>0.4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.70833333333333304</v>
       </c>
@@ -3627,9 +3909,19 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>0.6</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.75</v>
       </c>
@@ -3644,9 +3936,19 @@
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>0.7</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.79166666666666696</v>
       </c>
@@ -3661,9 +3963,19 @@
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>0.7</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0.83333333333333304</v>
       </c>
@@ -3678,9 +3990,19 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>0.6</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.875</v>
       </c>
@@ -3695,9 +4017,19 @@
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>0.7</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0.91666666666666696</v>
       </c>
@@ -3712,9 +4044,19 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>0.1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.95833333333333304</v>
       </c>
@@ -3729,7 +4071,17 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25">
+        <v>0.6</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added generic constraints for processes.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FF20ED-79B0-4E4A-990B-F58D1B33B255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4264FA4-91B3-4C57-85A4-A9E40CB129EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="scenarios" sheetId="9" r:id="rId11"/>
     <sheet name="fixed_ts" sheetId="11" r:id="rId12"/>
     <sheet name="eff_ts" sheetId="12" r:id="rId13"/>
+    <sheet name="constraints" sheetId="14" r:id="rId14"/>
+    <sheet name="gen_constraint" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
   <si>
     <t>node</t>
   </si>
@@ -333,6 +335,39 @@
   </si>
   <si>
     <t>is_cf_fix</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>c1,ngchp,elc,s1</t>
+  </si>
+  <si>
+    <t>c1,ngchp,elc,s2</t>
+  </si>
+  <si>
+    <t>c1,ngchp,elc,s3</t>
+  </si>
+  <si>
+    <t>c1,ngchp,dh,s1</t>
+  </si>
+  <si>
+    <t>c1,ngchp,dh,s2</t>
+  </si>
+  <si>
+    <t>c1,ngchp,dh,s3</t>
+  </si>
+  <si>
+    <t>c1,s1</t>
+  </si>
+  <si>
+    <t>c1,s2</t>
+  </si>
+  <si>
+    <t>c1,s3</t>
   </si>
 </sst>
 </file>
@@ -712,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,7 +2022,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2040,7 @@
         <v>49</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2021,7 +2056,7 @@
         <v>51</v>
       </c>
       <c r="B4">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -2542,12 +2577,858 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12AB76-2BDA-4ACA-A128-8CFB9FB6C8F8}">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>-0.8</v>
+      </c>
+      <c r="F2">
+        <v>-0.8</v>
+      </c>
+      <c r="G2">
+        <v>-0.8</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-0.8</v>
+      </c>
+      <c r="F3">
+        <v>-0.8</v>
+      </c>
+      <c r="G3">
+        <v>-0.8</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-0.8</v>
+      </c>
+      <c r="F4">
+        <v>-0.8</v>
+      </c>
+      <c r="G4">
+        <v>-0.8</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-0.8</v>
+      </c>
+      <c r="F5">
+        <v>-0.8</v>
+      </c>
+      <c r="G5">
+        <v>-0.8</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>-0.8</v>
+      </c>
+      <c r="F6">
+        <v>-0.8</v>
+      </c>
+      <c r="G6">
+        <v>-0.8</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>-0.8</v>
+      </c>
+      <c r="F7">
+        <v>-0.8</v>
+      </c>
+      <c r="G7">
+        <v>-0.8</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>-0.8</v>
+      </c>
+      <c r="F8">
+        <v>-0.8</v>
+      </c>
+      <c r="G8">
+        <v>-0.8</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>-0.8</v>
+      </c>
+      <c r="F9">
+        <v>-0.8</v>
+      </c>
+      <c r="G9">
+        <v>-0.8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>-0.8</v>
+      </c>
+      <c r="F10">
+        <v>-0.8</v>
+      </c>
+      <c r="G10">
+        <v>-0.8</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>-0.8</v>
+      </c>
+      <c r="F11">
+        <v>-0.8</v>
+      </c>
+      <c r="G11">
+        <v>-0.8</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>-0.8</v>
+      </c>
+      <c r="F12">
+        <v>-0.8</v>
+      </c>
+      <c r="G12">
+        <v>-0.8</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>-0.8</v>
+      </c>
+      <c r="F13">
+        <v>-0.8</v>
+      </c>
+      <c r="G13">
+        <v>-0.8</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>-0.8</v>
+      </c>
+      <c r="F14">
+        <v>-0.8</v>
+      </c>
+      <c r="G14">
+        <v>-0.8</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>-0.8</v>
+      </c>
+      <c r="F15">
+        <v>-0.8</v>
+      </c>
+      <c r="G15">
+        <v>-0.8</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>-0.8</v>
+      </c>
+      <c r="F16">
+        <v>-0.8</v>
+      </c>
+      <c r="G16">
+        <v>-0.8</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>-0.8</v>
+      </c>
+      <c r="F17">
+        <v>-0.8</v>
+      </c>
+      <c r="G17">
+        <v>-0.8</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>-0.8</v>
+      </c>
+      <c r="F18">
+        <v>-0.8</v>
+      </c>
+      <c r="G18">
+        <v>-0.8</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>-0.8</v>
+      </c>
+      <c r="F19">
+        <v>-0.8</v>
+      </c>
+      <c r="G19">
+        <v>-0.8</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>-0.8</v>
+      </c>
+      <c r="F20">
+        <v>-0.8</v>
+      </c>
+      <c r="G20">
+        <v>-0.8</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>-0.8</v>
+      </c>
+      <c r="F21">
+        <v>-0.8</v>
+      </c>
+      <c r="G21">
+        <v>-0.8</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>-0.8</v>
+      </c>
+      <c r="F22">
+        <v>-0.8</v>
+      </c>
+      <c r="G22">
+        <v>-0.8</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>-0.8</v>
+      </c>
+      <c r="F23">
+        <v>-0.8</v>
+      </c>
+      <c r="G23">
+        <v>-0.8</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>-0.8</v>
+      </c>
+      <c r="F24">
+        <v>-0.8</v>
+      </c>
+      <c r="G24">
+        <v>-0.8</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>-0.8</v>
+      </c>
+      <c r="F25">
+        <v>-0.8</v>
+      </c>
+      <c r="G25">
+        <v>-0.8</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,7 +3858,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4094,7 +4975,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4131,26 +5012,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <f>1*B2</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>1*C2</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3">
         <f>1*B2</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3">
         <f>1*C2</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed issue with ramp constraint. Added initial states for processes and for storages(states).
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4264FA4-91B3-4C57-85A4-A9E40CB129EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D945E25-DF45-41BF-B530-45D8A81DB053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="3" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
   <si>
     <t>node</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>c1,s3</t>
+  </si>
+  <si>
+    <t>initial_state</t>
   </si>
 </sst>
 </file>
@@ -745,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +767,7 @@
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -792,8 +795,11 @@
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -821,8 +827,11 @@
       <c r="I2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -850,8 +859,11 @@
       <c r="I3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -879,8 +891,11 @@
       <c r="I4" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -908,8 +923,11 @@
       <c r="I5" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -937,8 +955,11 @@
       <c r="I6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -964,6 +985,9 @@
         <v>0</v>
       </c>
       <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3425,10 +3449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,7 +3469,7 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -3482,8 +3506,11 @@
       <c r="L1" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3520,8 +3547,11 @@
       <c r="L2" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -3558,8 +3588,11 @@
       <c r="L3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -3596,8 +3629,11 @@
       <c r="L4" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -3634,8 +3670,11 @@
       <c r="L5" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -3672,8 +3711,11 @@
       <c r="L6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -3710,8 +3752,11 @@
       <c r="L7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3746,6 +3791,9 @@
         <v>0</v>
       </c>
       <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -3857,8 +3905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3920,10 +3968,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3946,10 +3994,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3972,10 +4020,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="6">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3998,10 +4046,10 @@
         <v>15</v>
       </c>
       <c r="G5" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4024,10 +4072,10 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4288,7 +4336,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4975,7 +5023,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5012,25 +5060,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E2">
         <f>1*C2</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="F2" s="3">
         <f>1*B2</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="G2" s="3">
         <f>1*C2</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrections and output methods
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Hope\Predicer_master\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D945E25-DF45-41BF-B530-45D8A81DB053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E35C52D-5BF9-4BB6-A864-5CB459C7E295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="3" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-46020" yWindow="780" windowWidth="21600" windowHeight="12735" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="eff_ts" sheetId="12" r:id="rId13"/>
     <sheet name="constraints" sheetId="14" r:id="rId14"/>
     <sheet name="gen_constraint" sheetId="15" r:id="rId15"/>
+    <sheet name="cap_ts" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="112">
   <si>
     <t>node</t>
   </si>
@@ -371,6 +372,18 @@
   </si>
   <si>
     <t>initial_state</t>
+  </si>
+  <si>
+    <t>hp1,elc,s1</t>
+  </si>
+  <si>
+    <t>hp1,elc,s2</t>
+  </si>
+  <si>
+    <t>hp1,elc,s3</t>
+  </si>
+  <si>
+    <t>state_loss</t>
   </si>
 </sst>
 </file>
@@ -748,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +780,7 @@
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -798,8 +811,11 @@
       <c r="J1" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -830,8 +846,11 @@
       <c r="J2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -862,8 +881,11 @@
       <c r="J3" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -892,10 +914,13 @@
         <v>3</v>
       </c>
       <c r="J4" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -926,8 +951,11 @@
       <c r="J5" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -958,8 +986,11 @@
       <c r="J6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -988,6 +1019,9 @@
         <v>0</v>
       </c>
       <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2637,7 +2671,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,6 +3474,371 @@
       </c>
       <c r="J25">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEDBA5-B0F3-4E9D-9367-08D5F5FA8AEA}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="B3">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="C3">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="D3">
+        <v>4.2857142857142856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="B4">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="C4">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="D4">
+        <v>4.2857142857142856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B5">
+        <v>4.4117647058823533</v>
+      </c>
+      <c r="C5">
+        <v>4.4117647058823533</v>
+      </c>
+      <c r="D5">
+        <v>4.4117647058823533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="B6">
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="C6">
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="D6">
+        <v>4.5454545454545459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="B7">
+        <v>4.6875</v>
+      </c>
+      <c r="C7">
+        <v>4.6875</v>
+      </c>
+      <c r="D7">
+        <v>4.6875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>4.838709677419355</v>
+      </c>
+      <c r="C8">
+        <v>4.838709677419355</v>
+      </c>
+      <c r="D8">
+        <v>4.838709677419355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="B19">
+        <v>3.75</v>
+      </c>
+      <c r="C19">
+        <v>3.75</v>
+      </c>
+      <c r="D19">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B20">
+        <v>3.75</v>
+      </c>
+      <c r="C20">
+        <v>3.75</v>
+      </c>
+      <c r="D20">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="B21">
+        <v>3.75</v>
+      </c>
+      <c r="C21">
+        <v>3.75</v>
+      </c>
+      <c r="D21">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="B22">
+        <v>3.75</v>
+      </c>
+      <c r="C22">
+        <v>3.75</v>
+      </c>
+      <c r="D22">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B23">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="C23">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="D23">
+        <v>4.2857142857142856</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="B24">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="C24">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="D24">
+        <v>4.2857142857142856</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B25">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="C25">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="D25">
+        <v>4.2857142857142856</v>
       </c>
     </row>
   </sheetData>
@@ -3452,7 +3851,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3905,7 +4304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improved the AbstractModel interface. Added functions to add Nodes and Processes in a smoother way. Changed "import_input_data.jl" to use these functions.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Hope\Predicer_master\Predicer\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E35C52D-5BF9-4BB6-A864-5CB459C7E295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0A4073-A20F-4529-8BD5-AB07D18B0824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46020" yWindow="780" windowWidth="21600" windowHeight="12735" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="6" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="G1:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5421,8 +5421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F87DD44-A1AD-4241-AED7-C48CC9DEE2E2}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed format of time stamps
Changed the format of the used timestamps to TimeZones.ZonedDateTime. Changed the input data in the input data file, and added TImeZones to the dependencies.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Hope\Predicer_master\Predicer\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer - Copy\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D377BFB-4D87-412E-8144-49501D205597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC4D9F8-212D-4541-B8DE-FD1C1A8E23AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="796" activeTab="10" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="10" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="117">
   <si>
     <t>node</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>state_loss</t>
+  </si>
+  <si>
+    <t>delay</t>
   </si>
   <si>
     <t>parameter</t>
@@ -403,6 +406,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy\ h:mm;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,9 +452,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,6 +465,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,7 +784,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="G1:K7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,38 +800,38 @@
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -832,34 +839,34 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8">
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -867,34 +874,34 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
         <v>0</v>
       </c>
     </row>
@@ -902,31 +909,31 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
         <v>10</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>3</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>3</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>10</v>
       </c>
       <c r="K4">
@@ -937,34 +944,34 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
         <v>4</v>
       </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8">
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
         <v>0</v>
       </c>
     </row>
@@ -972,34 +979,34 @@
       <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1007,34 +1014,34 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1048,59 +1055,60 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>48</v>
@@ -1140,8 +1148,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>60</v>
@@ -1181,8 +1189,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>58</v>
@@ -1222,8 +1230,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>51</v>
@@ -1263,8 +1271,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -1304,8 +1312,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>34</v>
@@ -1345,8 +1353,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>45</v>
@@ -1386,8 +1394,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>41</v>
@@ -1427,8 +1435,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>55</v>
@@ -1468,8 +1476,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>59</v>
@@ -1509,8 +1517,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>60</v>
@@ -1550,8 +1558,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>41</v>
@@ -1591,8 +1599,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>46</v>
@@ -1632,8 +1640,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>38</v>
@@ -1673,8 +1681,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>46</v>
@@ -1714,8 +1722,8 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -1755,8 +1763,8 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>41</v>
@@ -1796,8 +1804,8 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>46</v>
@@ -1837,8 +1845,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>52</v>
@@ -1878,8 +1886,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>56</v>
@@ -1919,8 +1927,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>33</v>
@@ -1960,8 +1968,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>43</v>
@@ -2001,8 +2009,8 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>57</v>
@@ -2042,8 +2050,8 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>32</v>
@@ -2089,11 +2097,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455BFA53-C3D0-4BC3-8FDD-0F1FF3FD2BAA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314D326-256A-435C-AAE3-3517FA836EAE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,16 +2110,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>113</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -2119,7 +2127,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -2140,11 +2148,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2182,141 +2190,144 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="B1:C12"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
+      <c r="A2" s="9">
+        <v>44671</v>
+      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="B3" s="3"/>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
+      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="B4" s="3"/>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
+      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="B6" s="3"/>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="B7" s="3"/>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="B8" s="3"/>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
+      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
     </row>
   </sheetData>
@@ -2329,28 +2340,31 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -2363,8 +2377,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>3.5</v>
@@ -2377,8 +2391,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>3.5</v>
@@ -2391,8 +2405,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>3.4</v>
@@ -2405,8 +2419,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>3.3</v>
@@ -2419,8 +2433,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>3.2</v>
@@ -2433,8 +2447,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>3.1</v>
@@ -2447,8 +2461,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2461,8 +2475,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>2.5</v>
@@ -2475,8 +2489,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>2.5</v>
@@ -2489,8 +2503,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>2.5</v>
@@ -2503,8 +2517,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>2.5</v>
@@ -2517,8 +2531,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>2.5</v>
@@ -2531,8 +2545,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>2.5</v>
@@ -2545,8 +2559,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>2.5</v>
@@ -2559,8 +2573,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>2.5</v>
@@ -2573,8 +2587,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>2.5</v>
@@ -2587,8 +2601,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2601,8 +2615,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2615,8 +2629,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2629,8 +2643,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -2643,8 +2657,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>3.5</v>
@@ -2657,8 +2671,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>3.5</v>
@@ -2671,8 +2685,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>3.5</v>
@@ -2730,6 +2744,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2764,8 +2781,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2796,8 +2813,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2828,8 +2845,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2860,8 +2877,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2892,8 +2909,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2924,8 +2941,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2956,8 +2973,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2988,8 +3005,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3020,8 +3037,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3052,8 +3069,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3084,8 +3101,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3116,8 +3133,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3148,8 +3165,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3180,8 +3197,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3212,8 +3229,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3244,8 +3261,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3276,8 +3293,8 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3308,8 +3325,8 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3340,8 +3357,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3372,8 +3389,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3404,8 +3421,8 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3436,8 +3453,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3468,8 +3485,8 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3500,8 +3517,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3541,10 +3558,13 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3561,8 +3581,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3575,8 +3595,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>4.2857142857142856</v>
@@ -3589,8 +3609,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>4.2857142857142856</v>
@@ -3603,8 +3623,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>4.4117647058823533</v>
@@ -3617,8 +3637,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>4.5454545454545459</v>
@@ -3631,8 +3651,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>4.6875</v>
@@ -3645,8 +3665,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>4.838709677419355</v>
@@ -3659,8 +3679,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -3673,8 +3693,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -3687,8 +3707,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -3701,8 +3721,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -3715,8 +3735,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -3729,8 +3749,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -3743,8 +3763,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -3757,8 +3777,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -3771,8 +3791,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -3785,8 +3805,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -3799,8 +3819,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>3.75</v>
@@ -3813,8 +3833,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>3.75</v>
@@ -3827,8 +3847,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>3.75</v>
@@ -3841,8 +3861,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>3.75</v>
@@ -3855,8 +3875,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>4.2857142857142856</v>
@@ -3869,8 +3889,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>4.2857142857142856</v>
@@ -3883,8 +3903,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>4.2857142857142856</v>
@@ -3903,15 +3923,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -3923,333 +3943,340 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="8">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8">
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7">
         <v>0.9</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>0.3</v>
       </c>
-      <c r="I2" s="8">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8">
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
         <v>4</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <v>3</v>
       </c>
-      <c r="M2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="7">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="8">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
         <v>3</v>
       </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
         <v>0.7</v>
       </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>1</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>0.99</v>
       </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0</v>
-      </c>
-      <c r="L7" s="8">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
         <v>3</v>
       </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
-        <v>0</v>
-      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4266,46 +4293,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4">
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
         <f>B1+1</f>
         <v>2</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <f t="shared" ref="D1:K1" si="0">C1+1</f>
         <v>3</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -4357,387 +4384,429 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="I1" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
         <v>20</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>3</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>0.5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
         <v>10</v>
       </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
         <v>0.5</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
         <v>0.5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
         <v>5</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>15</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0.5</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
         <v>15</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0.5</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>0.5</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
         <v>10</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>15</v>
       </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
         <v>7</v>
       </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
         <v>5</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>0.5</v>
       </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
         <v>5</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>0.5</v>
       </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
         <v>20</v>
       </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
         <v>20</v>
       </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1</v>
-      </c>
-      <c r="H14" s="6">
-        <v>1</v>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4751,16 +4820,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4787,40 +4856,43 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A4637A-7829-48D6-AE54-2E654AB1A427}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4846,8 +4918,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>0.4</v>
@@ -4873,8 +4945,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -4900,8 +4972,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4927,8 +4999,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>0.8</v>
@@ -4954,8 +5026,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4981,8 +5053,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>0.1</v>
@@ -5008,8 +5080,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>0.6</v>
@@ -5035,8 +5107,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>0.4</v>
@@ -5062,8 +5134,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>0.6</v>
@@ -5089,8 +5161,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>0.7</v>
@@ -5116,8 +5188,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>0.1</v>
@@ -5143,8 +5215,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>0.1</v>
@@ -5170,8 +5242,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>0.8</v>
@@ -5197,8 +5269,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>0.9</v>
@@ -5224,8 +5296,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>0.2</v>
@@ -5251,8 +5323,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>0.4</v>
@@ -5278,8 +5350,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>0.6</v>
@@ -5305,8 +5377,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>0.7</v>
@@ -5332,8 +5404,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>0.7</v>
@@ -5359,8 +5431,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>0.6</v>
@@ -5386,8 +5458,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>0.7</v>
@@ -5413,8 +5485,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>0.1</v>
@@ -5440,8 +5512,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>0.6</v>
@@ -5466,9 +5538,13 @@
         <v>0.6</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5477,41 +5553,42 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>-5</v>
@@ -5526,18 +5603,18 @@
         <f>1*C2</f>
         <v>-5</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <f>1*B2</f>
         <v>-5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <f>1*C2</f>
         <v>-5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>-5</v>
@@ -5553,18 +5630,18 @@
         <f t="shared" ref="E3:E25" si="1">1*C3</f>
         <v>-5</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f t="shared" ref="F3:F25" si="2">1*B3</f>
         <v>-5</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f t="shared" ref="G3:G25" si="3">1*C3</f>
         <v>-5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>-4</v>
@@ -5580,18 +5657,18 @@
         <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f t="shared" si="3"/>
         <v>-6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>-2</v>
@@ -5607,18 +5684,18 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" si="3"/>
         <v>-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>-7</v>
@@ -5634,18 +5711,18 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f t="shared" si="2"/>
         <v>-7</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" si="3"/>
         <v>-4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>-5</v>
@@ -5661,18 +5738,18 @@
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="3"/>
         <v>-5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>-14</v>
@@ -5688,18 +5765,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>-20</v>
@@ -5715,18 +5792,18 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="3"/>
         <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>-13</v>
@@ -5742,18 +5819,18 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <f t="shared" si="2"/>
         <v>-13</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f t="shared" si="3"/>
         <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>-12</v>
@@ -5769,18 +5846,18 @@
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <f t="shared" si="2"/>
         <v>-12</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <f t="shared" si="3"/>
         <v>-5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>-13</v>
@@ -5796,18 +5873,18 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <f t="shared" si="2"/>
         <v>-13</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <f t="shared" si="3"/>
         <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>-14</v>
@@ -5823,18 +5900,18 @@
         <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f t="shared" si="3"/>
         <v>-6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>-18</v>
@@ -5850,18 +5927,18 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f t="shared" si="2"/>
         <v>-18</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <f t="shared" si="3"/>
         <v>-4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>-14</v>
@@ -5877,18 +5954,18 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <f t="shared" si="3"/>
         <v>-3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>-15</v>
@@ -5904,18 +5981,18 @@
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <f t="shared" si="3"/>
         <v>-5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>-14</v>
@@ -5931,18 +6008,18 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>-20</v>
@@ -5958,18 +6035,18 @@
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <f t="shared" si="3"/>
         <v>-5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>-20</v>
@@ -5985,18 +6062,18 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <f t="shared" si="3"/>
         <v>-4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>-20</v>
@@ -6012,18 +6089,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>-20</v>
@@ -6039,18 +6116,18 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>-16</v>
@@ -6066,18 +6143,18 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <f t="shared" si="2"/>
         <v>-16</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <f t="shared" si="3"/>
         <v>-4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>-14</v>
@@ -6093,18 +6170,18 @@
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <f t="shared" si="3"/>
         <v>-5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>-11</v>
@@ -6120,18 +6197,18 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>-9</v>
@@ -6147,11 +6224,11 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <f t="shared" si="2"/>
         <v>-9</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <f t="shared" si="3"/>
         <v>-3</v>
       </c>
@@ -6168,28 +6245,31 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="9">
+        <v>44671</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -6202,8 +6282,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>4.1666666666666699E-2</v>
+      <c r="A3" s="9">
+        <v>44671.041666666664</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -6216,8 +6296,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>8.3333333333333301E-2</v>
+      <c r="A4" s="9">
+        <v>44671.08333321759</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -6230,8 +6310,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.125</v>
+      <c r="A5" s="9">
+        <v>44671.124999826388</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -6244,8 +6324,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.16666666666666699</v>
+      <c r="A6" s="9">
+        <v>44671.166666435187</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -6258,8 +6338,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.20833333333333301</v>
+      <c r="A7" s="9">
+        <v>44671.208333043978</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -6272,8 +6352,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.25</v>
+      <c r="A8" s="9">
+        <v>44671.249999652777</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -6286,8 +6366,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.29166666666666702</v>
+      <c r="A9" s="9">
+        <v>44671.291666261575</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -6300,8 +6380,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.33333333333333298</v>
+      <c r="A10" s="9">
+        <v>44671.333332870374</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -6314,8 +6394,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.375</v>
+      <c r="A11" s="9">
+        <v>44671.374999479165</v>
       </c>
       <c r="B11">
         <v>12</v>
@@ -6328,8 +6408,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.41666666666666702</v>
+      <c r="A12" s="9">
+        <v>44671.416666087964</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -6342,8 +6422,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.45833333333333298</v>
+      <c r="A13" s="9">
+        <v>44671.458332696762</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -6356,8 +6436,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.5</v>
+      <c r="A14" s="9">
+        <v>44671.499999305554</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -6370,8 +6450,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.54166666666666696</v>
+      <c r="A15" s="9">
+        <v>44671.541665914352</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -6384,8 +6464,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.58333333333333304</v>
+      <c r="A16" s="9">
+        <v>44671.583332523151</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -6398,8 +6478,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.625</v>
+      <c r="A17" s="9">
+        <v>44671.624999131942</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -6412,8 +6492,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.66666666666666696</v>
+      <c r="A18" s="9">
+        <v>44671.66666574074</v>
       </c>
       <c r="B18">
         <v>12</v>
@@ -6426,8 +6506,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.70833333333333304</v>
+      <c r="A19" s="9">
+        <v>44671.708332349539</v>
       </c>
       <c r="B19">
         <v>12</v>
@@ -6440,8 +6520,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.75</v>
+      <c r="A20" s="9">
+        <v>44671.74999895833</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -6454,8 +6534,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.79166666666666696</v>
+      <c r="A21" s="9">
+        <v>44671.791665567129</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -6468,8 +6548,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.83333333333333304</v>
+      <c r="A22" s="9">
+        <v>44671.833332175927</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -6482,8 +6562,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.875</v>
+      <c r="A23" s="9">
+        <v>44671.874998784719</v>
       </c>
       <c r="B23">
         <v>12</v>
@@ -6496,8 +6576,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.91666666666666696</v>
+      <c r="A24" s="9">
+        <v>44671.916665393517</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -6510,8 +6590,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.95833333333333304</v>
+      <c r="A25" s="9">
+        <v>44671.958332002316</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -6542,107 +6622,107 @@
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="8">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>0.2</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>0.2</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added structs for input data and time structure.
Added struct 'InputData', which is used to store the defined data which the model is built on. A set format for the input data makes it easier to assure the validity and consistency of the data.

Also added the struct 'Temporals', which stores the timesteps in the model, as well as information on the length between timesteps.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer - Copy\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC4D9F8-212D-4541-B8DE-FD1C1A8E23AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8968EC7D-612A-45C5-959A-A6805E912DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="10" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="8" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="118">
   <si>
     <t>node</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>is_bid</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314D326-256A-435C-AAE3-3517FA836EAE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -6610,10 +6613,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3788A93-7501-4F5D-9E8F-38D329CC85EC}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6626,7 +6629,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -6645,8 +6648,11 @@
       <c r="F1" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -6665,8 +6671,11 @@
       <c r="F2" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -6685,8 +6694,11 @@
       <c r="F3" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -6705,8 +6717,11 @@
       <c r="F4" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -6724,6 +6739,9 @@
       </c>
       <c r="F5" s="7" t="s">
         <v>87</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved model time structure
Added the field "ts_format" to the Temporals struct, and changed code to use this format.

Changed how TimeSeries and TimeSeriesData can be called to retrieve the value of a specific timestamp.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE149ADE-FA06-4FED-B224-E237691D8654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA097E-C4A6-4A19-890A-D9512F462D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-57720" yWindow="-3360" windowWidth="29040" windowHeight="17640" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -787,7 +787,7 @@
   <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2205,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed how the timesteps are imported
Changed the temporals to be directly defined in the input data file, instead of being scraped together from each defined timeseries.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA097E-C4A6-4A19-890A-D9512F462D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F5F1FB-53C3-4C42-9D35-A7A06F9EF485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-3360" windowWidth="29040" windowHeight="17640" tabRatio="796" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
   <si>
     <t>node</t>
   </si>
@@ -385,25 +385,25 @@
     <t>hp1,elc,s3</t>
   </si>
   <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>alfa</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>is_bid</t>
+  </si>
+  <si>
     <t>state_loss</t>
-  </si>
-  <si>
-    <t>delay</t>
-  </si>
-  <si>
-    <t>parameter</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>alfa</t>
-  </si>
-  <si>
-    <t>beta</t>
-  </si>
-  <si>
-    <t>is_bid</t>
   </si>
 </sst>
 </file>
@@ -784,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39053E69-3A75-490E-847C-66A9CF6C1FC5}">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,127 +796,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8">
-        <v>44671</v>
+      <c r="A1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>44671.041666666664</v>
+        <v>44671</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>44671.08333321759</v>
+        <v>44671.041666666664</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>44671.124999826388</v>
+        <v>44671.08333321759</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>44671.166666435187</v>
+        <v>44671.124999826388</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>44671.208333043978</v>
+        <v>44671.166666435187</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>44671.249999652777</v>
+        <v>44671.208333043978</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>44671.291666261575</v>
+        <v>44671.249999652777</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>44671.333332870374</v>
+        <v>44671.291666261575</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>44671.374999479165</v>
+        <v>44671.333332870374</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>44671.416666087964</v>
+        <v>44671.374999479165</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>44671.458332696762</v>
+        <v>44671.416666087964</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>44671.499999305554</v>
+        <v>44671.458332696762</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>44671.541665914352</v>
+        <v>44671.499999305554</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>44671.583332523151</v>
+        <v>44671.541665914352</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>44671.624999131942</v>
+        <v>44671.583332523151</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>44671.66666574074</v>
+        <v>44671.624999131942</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>44671.708332349539</v>
+        <v>44671.66666574074</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>44671.74999895833</v>
+        <v>44671.708332349539</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>44671.791665567129</v>
+        <v>44671.74999895833</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>44671.833332175927</v>
+        <v>44671.791665567129</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>44671.874998784719</v>
+        <v>44671.833332175927</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>44671.916665393517</v>
+        <v>44671.874998784719</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
+        <v>44671.916665393517</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
         <v>44671.958332002316</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
@@ -986,6 +988,9 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1030,7 +1035,7 @@
         <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1188,7 +1193,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -1230,7 +1235,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -1272,7 +1277,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -1314,7 +1319,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -1356,7 +1361,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -1398,7 +1403,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -1440,7 +1445,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -1482,7 +1487,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -1524,7 +1529,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -1566,7 +1571,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -1608,7 +1613,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -1650,7 +1655,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -1692,7 +1697,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -1734,7 +1739,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -1776,7 +1781,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -1818,7 +1823,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -1860,7 +1865,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -1902,7 +1907,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -1944,7 +1949,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -1986,7 +1991,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -2028,7 +2033,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -2070,7 +2075,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -2112,7 +2117,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -2154,7 +2159,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
@@ -2215,15 +2220,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -2231,7 +2236,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -2309,152 +2314,152 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
     </row>
@@ -2492,7 +2497,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -2507,7 +2512,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -2522,7 +2527,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -2537,7 +2542,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -2552,7 +2557,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -2567,7 +2572,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -2582,7 +2587,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -2597,7 +2602,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -2612,7 +2617,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -2627,7 +2632,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -2642,7 +2647,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -2657,7 +2662,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -2672,7 +2677,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -2687,7 +2692,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -2702,7 +2707,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -2717,7 +2722,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -2732,7 +2737,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -2747,7 +2752,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -2762,7 +2767,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -2777,7 +2782,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -2792,7 +2797,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -2807,7 +2812,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -2822,7 +2827,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -2837,7 +2842,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
@@ -2934,7 +2939,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -2967,7 +2972,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -3000,7 +3005,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -3033,7 +3038,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -3066,7 +3071,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -3099,7 +3104,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -3132,7 +3137,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -3165,7 +3170,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -3198,7 +3203,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -3231,7 +3236,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -3264,7 +3269,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -3297,7 +3302,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -3330,7 +3335,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -3363,7 +3368,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -3396,7 +3401,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -3429,7 +3434,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -3462,7 +3467,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -3495,7 +3500,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -3528,7 +3533,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -3561,7 +3566,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -3594,7 +3599,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -3627,7 +3632,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -3660,7 +3665,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -3693,7 +3698,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
@@ -3758,7 +3763,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -3773,7 +3778,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -3788,7 +3793,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -3803,7 +3808,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -3818,7 +3823,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -3833,7 +3838,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -3848,7 +3853,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -3863,7 +3868,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -3878,7 +3883,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -3893,7 +3898,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -3908,7 +3913,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -3923,7 +3928,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -3938,7 +3943,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -3953,7 +3958,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -3968,7 +3973,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -3983,7 +3988,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -3998,7 +4003,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -4013,7 +4018,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -4028,7 +4033,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -4043,7 +4048,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -4058,7 +4063,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -4073,7 +4078,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -4088,7 +4093,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -4103,7 +4108,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
@@ -4123,10 +4128,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,7 +4147,7 @@
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4174,10 +4179,10 @@
         <v>107</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4211,8 +4216,9 @@
       <c r="K2" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4246,8 +4252,9 @@
       <c r="K3" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4281,8 +4288,9 @@
       <c r="K4">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4316,8 +4324,9 @@
       <c r="K5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -4351,8 +4360,9 @@
       <c r="K6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4386,6 +4396,7 @@
       <c r="K7" s="7">
         <v>0</v>
       </c>
+      <c r="L7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4900,7 +4911,7 @@
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5365,7 +5376,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -5394,7 +5405,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -5422,7 +5433,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -5450,7 +5461,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -5478,7 +5489,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -5506,7 +5517,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -5534,7 +5545,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -5562,7 +5573,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -5590,7 +5601,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -5618,7 +5629,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -5646,7 +5657,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -5674,7 +5685,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -5702,7 +5713,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -5730,7 +5741,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -5758,7 +5769,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -5786,7 +5797,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -5814,7 +5825,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -5842,7 +5853,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -5870,7 +5881,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -5898,7 +5909,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -5926,7 +5937,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -5954,7 +5965,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -5982,7 +5993,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -6010,7 +6021,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
@@ -6083,7 +6094,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -6110,7 +6121,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -6138,7 +6149,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -6166,7 +6177,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -6194,7 +6205,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -6222,7 +6233,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -6250,7 +6261,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -6278,7 +6289,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -6306,7 +6317,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -6334,7 +6345,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -6362,7 +6373,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -6390,7 +6401,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -6418,7 +6429,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -6446,7 +6457,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -6474,7 +6485,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -6502,7 +6513,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -6530,7 +6541,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -6558,7 +6569,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -6586,7 +6597,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -6614,7 +6625,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -6642,7 +6653,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -6670,7 +6681,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -6698,7 +6709,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -6726,7 +6737,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
@@ -6788,7 +6799,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>IF(timeseries!A1&lt;&gt;"",timeseries!A1,"")</f>
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2">
@@ -6803,7 +6814,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3">
@@ -6818,7 +6829,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4">
@@ -6833,7 +6844,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5">
@@ -6848,7 +6859,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6">
@@ -6863,7 +6874,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7">
@@ -6878,7 +6889,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8">
@@ -6893,7 +6904,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
       <c r="B9">
@@ -6908,7 +6919,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
       <c r="B10">
@@ -6923,7 +6934,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
       <c r="B11">
@@ -6938,7 +6949,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
       <c r="B12">
@@ -6953,7 +6964,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
       <c r="B13">
@@ -6968,7 +6979,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
       <c r="B14">
@@ -6983,7 +6994,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
       <c r="B15">
@@ -6998,7 +7009,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
       <c r="B16">
@@ -7013,7 +7024,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
       <c r="B17">
@@ -7028,7 +7039,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
       <c r="B18">
@@ -7043,7 +7054,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
       <c r="B19">
@@ -7058,7 +7069,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
       <c r="B20">
@@ -7073,7 +7084,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
       <c r="B21">
@@ -7088,7 +7099,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
       <c r="B22">
@@ -7103,7 +7114,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
       <c r="B23">
@@ -7118,7 +7129,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
       <c r="B24">
@@ -7133,7 +7144,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">

</xml_diff>

<commit_message>
Changed state loss parameter name
Changed the state_loss field in the State struct to state_loss_proportional, to better describe the functionality.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F5F1FB-53C3-4C42-9D35-A7A06F9EF485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EC21E0-C1A8-4BAE-A489-428689C8CAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
@@ -403,7 +403,7 @@
     <t>is_bid</t>
   </si>
   <si>
-    <t>state_loss</t>
+    <t>state_loss_proportional</t>
   </si>
 </sst>
 </file>
@@ -4131,7 +4131,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed timeseries inputdata in regards to scenarios.
TimeSeries data, such as inflows or prices, can now be defined for several or all scenarios. This reduces clutter in the input_data file.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EC21E0-C1A8-4BAE-A489-428689C8CAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639541A3-9B13-4CDF-A7F9-3FA28E4677D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-28920" yWindow="-3210" windowWidth="29040" windowHeight="17640" tabRatio="796" firstSheet="6" activeTab="8" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="134">
   <si>
     <t>node</t>
   </si>
@@ -235,15 +235,6 @@
     <t>h2,s3</t>
   </si>
   <si>
-    <t>ng,s1</t>
-  </si>
-  <si>
-    <t>ng,s2</t>
-  </si>
-  <si>
-    <t>ng,s3</t>
-  </si>
-  <si>
     <t>npe,s1</t>
   </si>
   <si>
@@ -404,6 +395,63 @@
   </si>
   <si>
     <t>state_loss_proportional</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>is_limited</t>
+  </si>
+  <si>
+    <t>limited_by</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>flow</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>constant_diff</t>
+  </si>
+  <si>
+    <t>flow_val</t>
+  </si>
+  <si>
+    <t>state_val</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>timeseries</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>c1, s1</t>
+  </si>
+  <si>
+    <t>ng, ALL</t>
   </si>
 </sst>
 </file>
@@ -1029,13 +1077,13 @@
         <v>44</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1095,13 +1143,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E4" s="7">
         <v>0.2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1118,13 +1166,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" s="7">
         <v>0.2</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1155,40 +1203,40 @@
         <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2220,15 +2268,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -2236,7 +2284,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -2486,13 +2534,13 @@
         <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2863,15 +2911,19 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -2879,12 +2931,114 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2896,8 +3050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12AB76-2BDA-4ACA-A128-8CFB9FB6C8F8}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2910,31 +3064,31 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3752,13 +3906,13 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4130,7 +4284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -4176,10 +4330,10 @@
         <v>5</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4433,7 +4587,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -4454,16 +4608,16 @@
         <v>19</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -4636,7 +4790,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -4821,7 +4975,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B2">
         <v>0.4</v>
@@ -4841,7 +4995,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <v>0.8</v>
@@ -4911,7 +5065,7 @@
         <v>21</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5148,7 +5302,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>30</v>
@@ -5312,12 +5466,12 @@
         <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -5325,7 +5479,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5364,13 +5518,13 @@
         <v>54</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H1"/>
     </row>
@@ -6772,10 +6926,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02307C1F-427B-487D-B703-EBF512D7AC27}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6783,21 +6937,15 @@
     <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -6805,14 +6953,8 @@
       <c r="B2">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -6820,14 +6962,8 @@
       <c r="B3">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -6835,14 +6971,8 @@
       <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -6850,14 +6980,8 @@
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -6865,14 +6989,8 @@
       <c r="B6">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -6880,14 +6998,8 @@
       <c r="B7">
         <v>12</v>
       </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -6895,14 +7007,8 @@
       <c r="B8">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -6910,14 +7016,8 @@
       <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -6925,14 +7025,8 @@
       <c r="B10">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -6940,14 +7034,8 @@
       <c r="B11">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -6955,14 +7043,8 @@
       <c r="B12">
         <v>12</v>
       </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -6970,14 +7052,8 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -6985,14 +7061,8 @@
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -7000,14 +7070,8 @@
       <c r="B15">
         <v>12</v>
       </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -7015,14 +7079,8 @@
       <c r="B16">
         <v>12</v>
       </c>
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -7030,14 +7088,8 @@
       <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -7045,14 +7097,8 @@
       <c r="B18">
         <v>12</v>
       </c>
-      <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -7060,14 +7106,8 @@
       <c r="B19">
         <v>12</v>
       </c>
-      <c r="C19">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -7075,14 +7115,8 @@
       <c r="B20">
         <v>12</v>
       </c>
-      <c r="C20">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -7090,14 +7124,8 @@
       <c r="B21">
         <v>12</v>
       </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -7105,14 +7133,8 @@
       <c r="B22">
         <v>12</v>
       </c>
-      <c r="C22">
-        <v>12</v>
-      </c>
-      <c r="D22">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -7120,14 +7142,8 @@
       <c r="B23">
         <v>12</v>
       </c>
-      <c r="C23">
-        <v>12</v>
-      </c>
-      <c r="D23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -7135,25 +7151,13 @@
       <c r="B24">
         <v>12</v>
       </c>
-      <c r="C24">
-        <v>12</v>
-      </c>
-      <c r="D24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
       </c>
       <c r="B25">
-        <v>12</v>
-      </c>
-      <c r="C25">
-        <v>12</v>
-      </c>
-      <c r="D25">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added input data check before model is compiled
Added functionality to check the validity of the given input data before the model is built. Additional checks will likely surface later, and the validation will have to be updated accordingly.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94084F68-772D-43D8-9564-7383FB110EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDF90C4-4951-4B86-BEF3-B6CC9900F6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3210" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="15" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -2290,7 +2290,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,7 +2856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4134,7 +4134,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,8 +4410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added residual costs to states
Added functionality to take into account the value of the states (storages) at the end of the optimization. The value per unit can be defined in the input data. If the defined value is positive, the contents of the state is calculated as a "gain", if negative, as a "loss".
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDF90C4-4951-4B86-BEF3-B6CC9900F6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27E139A-364B-4942-9AFD-1E9D13EDE797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
   <si>
     <t>node</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>pv1,s1,s2,s3</t>
+  </si>
+  <si>
+    <t>residual_value</t>
   </si>
 </sst>
 </file>
@@ -4133,8 +4136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,6 +4187,9 @@
       <c r="K1" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4219,7 +4225,9 @@
       <c r="K2" s="7">
         <v>0</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4255,7 +4263,9 @@
       <c r="K3" s="7">
         <v>0</v>
       </c>
-      <c r="L3" s="7"/>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4291,7 +4301,9 @@
       <c r="K4">
         <v>1E-3</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4327,7 +4339,9 @@
       <c r="K5" s="7">
         <v>0</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="7">
+        <v>1000</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4363,7 +4377,9 @@
       <c r="K6" s="7">
         <v>0</v>
       </c>
-      <c r="L6" s="7"/>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -4399,7 +4415,9 @@
       <c r="K7" s="7">
         <v>0</v>
       </c>
-      <c r="L7" s="7"/>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4410,7 +4428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added functionality for process delays.
Added functionality for having delays over processes.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27E139A-364B-4942-9AFD-1E9D13EDE797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6342B90-F8EE-4C3F-8710-409C3F73327A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" firstSheet="2" activeTab="4" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -18,19 +18,20 @@
     <sheet name="processes" sheetId="2" r:id="rId3"/>
     <sheet name="efficiencies" sheetId="10" r:id="rId4"/>
     <sheet name="process_topology" sheetId="6" r:id="rId5"/>
-    <sheet name="reserve_type" sheetId="13" r:id="rId6"/>
-    <sheet name="cf" sheetId="7" r:id="rId7"/>
-    <sheet name="inflow" sheetId="3" r:id="rId8"/>
-    <sheet name="price" sheetId="4" r:id="rId9"/>
-    <sheet name="markets" sheetId="5" r:id="rId10"/>
-    <sheet name="market_prices" sheetId="8" r:id="rId11"/>
-    <sheet name="risk" sheetId="17" r:id="rId12"/>
-    <sheet name="scenarios" sheetId="9" r:id="rId13"/>
-    <sheet name="fixed_ts" sheetId="11" r:id="rId14"/>
-    <sheet name="eff_ts" sheetId="12" r:id="rId15"/>
-    <sheet name="constraints" sheetId="14" r:id="rId16"/>
-    <sheet name="gen_constraint" sheetId="15" r:id="rId17"/>
-    <sheet name="cap_ts" sheetId="16" r:id="rId18"/>
+    <sheet name="node_history" sheetId="19" r:id="rId6"/>
+    <sheet name="reserve_type" sheetId="13" r:id="rId7"/>
+    <sheet name="cf" sheetId="7" r:id="rId8"/>
+    <sheet name="inflow" sheetId="3" r:id="rId9"/>
+    <sheet name="price" sheetId="4" r:id="rId10"/>
+    <sheet name="markets" sheetId="5" r:id="rId11"/>
+    <sheet name="market_prices" sheetId="8" r:id="rId12"/>
+    <sheet name="risk" sheetId="17" r:id="rId13"/>
+    <sheet name="scenarios" sheetId="9" r:id="rId14"/>
+    <sheet name="fixed_ts" sheetId="11" r:id="rId15"/>
+    <sheet name="eff_ts" sheetId="12" r:id="rId16"/>
+    <sheet name="constraints" sheetId="14" r:id="rId17"/>
+    <sheet name="gen_constraint" sheetId="15" r:id="rId18"/>
+    <sheet name="cap_ts" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="116">
   <si>
     <t>node</t>
   </si>
@@ -781,7 +782,7 @@
   <dimension ref="A1:A49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,6 +993,248 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02307C1F-427B-487D-B703-EBF512D7AC27}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <v>44671</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <v>44671.041666666664</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <v>44671.08333321759</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <v>44671.124999826388</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <v>44671.166666435187</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <v>44671.208333043978</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <v>44671.249999652777</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <v>44671.291666261575</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <v>44671.333332870374</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <v>44671.374999479165</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <v>44671.416666087964</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <v>44671.458332696762</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <v>44671.499999305554</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <v>44671.541665914352</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <v>44671.583332523151</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <v>44671.624999131942</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <v>44671.66666574074</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <v>44671.708332349539</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <v>44671.74999895833</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <v>44671.791665567129</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <v>44671.833332175927</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <v>44671.874998784719</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <v>44671.916665393517</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
+        <v>44671.958332002316</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3788A93-7501-4F5D-9E8F-38D329CC85EC}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -1129,12 +1372,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DDD9A-EF34-4108-8532-230729E9C708}">
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,7 +2442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314D326-256A-435C-AAE3-3517FA836EAE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2241,7 +2484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87AD413-E614-48C1-80E1-F1E8236FCBC6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2288,7 +2531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31679CA5-0AA2-4F6F-8223-14BF74917F04}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -2462,7 +2705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD670E02-665B-45B8-BC4E-9596D2C1BC55}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -2855,7 +3098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -2897,18 +3140,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE12AB76-2BDA-4ACA-A128-8CFB9FB6C8F8}">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-    <col min="2" max="10" width="2.28515625" customWidth="1"/>
+    <col min="2" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3740,12 +3985,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FEDBA5-B0F3-4E9D-9367-08D5F5FA8AEA}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,8 +4381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="7">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4429,7 +4674,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G2" sqref="G2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,8 +5134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5319,6 +5564,179 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AEF404-3743-47D7-AC45-7AE3A9FB796E}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
+        <v>44671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
+        <v>44671.041666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
+        <v>44671.08333321759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
+        <v>44671.124999826388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
+        <v>44671.166666435187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
+        <v>44671.208333043978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
+        <v>44671.249999652777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
+        <v>44671.291666261575</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
+        <v>44671.333332870374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
+        <v>44671.374999479165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
+        <v>44671.416666087964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
+        <v>44671.458332696762</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
+        <v>44671.499999305554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
+        <v>44671.541665914352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
+        <v>44671.583332523151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
+        <v>44671.624999131942</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
+        <v>44671.66666574074</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
+        <v>44671.708332349539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
+        <v>44671.74999895833</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
+        <v>44671.791665567129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
+        <v>44671.833332175927</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
+        <v>44671.874998784719</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
+        <v>44671.916665393517</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
+        <v>44671.958332002316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0532F8A-0FB4-47AD-98A1-4065D3376432}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -5357,7 +5775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A4637A-7829-48D6-AE54-2E654AB1A427}">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -5879,12 +6297,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F87DD44-A1AD-4241-AED7-C48CC9DEE2E2}">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6593,246 +7011,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02307C1F-427B-487D-B703-EBF512D7AC27}">
-  <dimension ref="A1:B25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
-        <v>44671</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
-        <v>44671.041666666664</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
-        <v>44671.124999826388</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
-        <v>44671.166666435187</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
-        <v>44671.208333043978</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
-        <v>44671.249999652777</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
-        <v>44671.291666261575</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
-        <v>44671.333332870374</v>
-      </c>
-      <c r="B10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
-        <v>44671.374999479165</v>
-      </c>
-      <c r="B11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
-        <v>44671.416666087964</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
-        <v>44671.458332696762</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
-        <v>44671.499999305554</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
-        <v>44671.541665914352</v>
-      </c>
-      <c r="B15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
-        <v>44671.583332523151</v>
-      </c>
-      <c r="B16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
-        <v>44671.624999131942</v>
-      </c>
-      <c r="B17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
-        <v>44671.66666574074</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
-        <v>44671.708332349539</v>
-      </c>
-      <c r="B19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
-        <v>44671.74999895833</v>
-      </c>
-      <c r="B20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
-        <v>44671.791665567129</v>
-      </c>
-      <c r="B21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
-        <v>44671.833332175927</v>
-      </c>
-      <c r="B22">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
-        <v>44671.874998784719</v>
-      </c>
-      <c r="B23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
-        <v>44671.916665393517</v>
-      </c>
-      <c r="B24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
-        <v>44671.958332002316</v>
-      </c>
-      <c r="B25">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified input data files
Added option to define maximum online and offline times in the input data. if the value is set to 0.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253483F0-6DED-4DE5-B58F-3DE617FDF60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4CC0F0-015F-4206-A7B8-98400E5BF38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18240" windowHeight="28440" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="124">
   <si>
     <t>node</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>npe,dw,s3</t>
+  </si>
+  <si>
+    <t>max_online</t>
+  </si>
+  <si>
+    <t>max_offline</t>
   </si>
 </sst>
 </file>
@@ -804,206 +810,206 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44671.249999652777</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44671.291666261575</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44671.333332870374</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44671.374999479165</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>44671.416666087964</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>44671.458332696762</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>44671.499999305554</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>44671.541665914352</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>44671.583332523151</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>44671.624999131942</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>44671.66666574074</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>44671.708332349539</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>44671.74999895833</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>44671.791665567129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>44671.833332175927</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>44671.874998784719</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>44671.916665393517</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>44671.958332002316</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
     </row>
   </sheetData>
@@ -1019,12 +1025,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -1041,7 +1047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -1050,7 +1056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -1059,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -1068,7 +1074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -1077,7 +1083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -1086,7 +1092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -1095,7 +1101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -1104,7 +1110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -1113,7 +1119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -1122,7 +1128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -1131,7 +1137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -1140,7 +1146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -1149,7 +1155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -1158,7 +1164,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -1167,7 +1173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -1176,7 +1182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -1185,7 +1191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -1194,7 +1200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -1203,7 +1209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -1212,7 +1218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -1221,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -1230,7 +1236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -1239,7 +1245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -1261,17 +1267,17 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>43</v>
       </c>
@@ -1399,14 +1405,14 @@
       <selection activeCell="M2" sqref="M2:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="2" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="13" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="2" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1447,7 +1453,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -1489,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -1531,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -1573,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -1615,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -1657,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -1699,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -1741,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -1783,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -1825,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -1867,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -1909,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -1951,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -1993,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -2035,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -2077,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -2119,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -2161,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -2203,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -2245,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -2287,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -2329,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -2371,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -2413,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -2469,14 +2475,14 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="7" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -2529,7 +2535,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -2559,7 +2565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -2589,7 +2595,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -2619,7 +2625,7 @@
         <v>22.95</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -2649,7 +2655,7 @@
         <v>16.650000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -2679,7 +2685,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -2709,7 +2715,7 @@
         <v>20.25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -2739,7 +2745,7 @@
         <v>18.45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -2769,7 +2775,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -2799,7 +2805,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -2829,7 +2835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -2859,7 +2865,7 @@
         <v>18.45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -2889,7 +2895,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -2919,7 +2925,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -2949,7 +2955,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -2979,7 +2985,7 @@
         <v>20.25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -3009,7 +3015,7 @@
         <v>18.45</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -3039,7 +3045,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -3069,7 +3075,7 @@
         <v>23.400000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -3099,7 +3105,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -3129,7 +3135,7 @@
         <v>14.85</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -3159,7 +3165,7 @@
         <v>19.350000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -3189,7 +3195,7 @@
         <v>25.650000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -3233,12 +3239,12 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>106</v>
       </c>
@@ -3246,7 +3252,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -3254,7 +3260,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3275,9 +3281,9 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -3285,7 +3291,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -3293,7 +3299,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -3301,7 +3307,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -3322,162 +3328,162 @@
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -3496,12 +3502,12 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -3515,7 +3521,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -3530,7 +3536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -3545,7 +3551,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -3560,7 +3566,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -3575,7 +3581,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -3590,7 +3596,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -3605,7 +3611,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -3620,7 +3626,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -3635,7 +3641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -3650,7 +3656,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -3665,7 +3671,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -3680,7 +3686,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -3695,7 +3701,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -3710,7 +3716,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -3725,7 +3731,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -3740,7 +3746,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -3755,7 +3761,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -3770,7 +3776,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -3785,7 +3791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -3800,7 +3806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -3815,7 +3821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -3830,7 +3836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -3845,7 +3851,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -3860,7 +3866,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -3889,14 +3895,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -3904,7 +3910,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -3912,7 +3918,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -3931,15 +3937,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="2" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="2" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -4004,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -4037,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -4070,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -4103,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -4136,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -4169,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -4202,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -4235,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -4268,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -4301,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -4334,7 +4340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -4367,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -4400,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -4433,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -4466,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -4499,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -4532,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -4565,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -4598,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -4631,7 +4637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -4664,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -4697,7 +4703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -4730,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -4776,20 +4782,20 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4827,7 +4833,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4865,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4903,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4941,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4979,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -5017,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5068,12 +5074,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -5087,7 +5093,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -5102,7 +5108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -5117,7 +5123,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -5132,7 +5138,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -5147,7 +5153,7 @@
         <v>4.4117647058823533</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -5162,7 +5168,7 @@
         <v>4.5454545454545459</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -5177,7 +5183,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -5192,7 +5198,7 @@
         <v>4.838709677419355</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -5207,7 +5213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -5222,7 +5228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -5237,7 +5243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -5252,7 +5258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -5267,7 +5273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -5282,7 +5288,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -5297,7 +5303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -5312,7 +5318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -5327,7 +5333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -5342,7 +5348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -5357,7 +5363,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -5372,7 +5378,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -5387,7 +5393,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -5402,7 +5408,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -5417,7 +5423,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -5432,7 +5438,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -5454,27 +5460,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -5512,13 +5519,19 @@
         <v>76</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -5556,13 +5569,19 @@
         <v>3</v>
       </c>
       <c r="M2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="7">
+        <v>1</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -5605,8 +5624,14 @@
       <c r="N3" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="7">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -5649,8 +5674,14 @@
       <c r="N4" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -5693,8 +5724,14 @@
       <c r="N5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -5737,8 +5774,14 @@
       <c r="N6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -5781,8 +5824,14 @@
       <c r="N7" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -5823,6 +5872,12 @@
         <v>0</v>
       </c>
       <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
         <v>0</v>
       </c>
     </row>
@@ -5839,9 +5894,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -5885,7 +5940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5905,7 +5960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -5938,20 +5993,20 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -5977,7 +6032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -6003,7 +6058,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -6029,7 +6084,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -6055,7 +6110,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -6081,7 +6136,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -6107,7 +6162,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -6133,7 +6188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -6159,7 +6214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -6185,7 +6240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
@@ -6211,7 +6266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
@@ -6237,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -6263,7 +6318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -6289,7 +6344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -6329,12 +6384,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -6345,145 +6400,145 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -6502,9 +6557,9 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -6512,7 +6567,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -6520,7 +6575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -6541,14 +6596,14 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -6566,7 +6621,7 @@
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -6588,7 +6643,7 @@
       <c r="F2" s="8"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -6608,7 +6663,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -6628,7 +6683,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -6648,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -6668,7 +6723,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -6688,7 +6743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -6708,7 +6763,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -6728,7 +6783,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -6748,7 +6803,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -6768,7 +6823,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -6788,7 +6843,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -6808,7 +6863,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -6828,7 +6883,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -6848,7 +6903,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -6868,7 +6923,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -6888,7 +6943,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -6908,7 +6963,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -6928,7 +6983,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -6948,7 +7003,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -6968,7 +7023,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -6988,7 +7043,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -7008,7 +7063,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -7028,7 +7083,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>
@@ -7063,14 +7118,14 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="8" customWidth="1"/>
-    <col min="4" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="4" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -7093,7 +7148,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -7120,7 +7175,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -7148,7 +7203,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -7176,7 +7231,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -7204,7 +7259,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -7232,7 +7287,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v>44671.208333043978</v>
@@ -7260,7 +7315,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v>44671.249999652777</v>
@@ -7288,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v>44671.291666261575</v>
@@ -7316,7 +7371,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v>44671.333332870374</v>
@@ -7344,7 +7399,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v>44671.374999479165</v>
@@ -7372,7 +7427,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v>44671.416666087964</v>
@@ -7400,7 +7455,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v>44671.458332696762</v>
@@ -7428,7 +7483,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v>44671.499999305554</v>
@@ -7456,7 +7511,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v>44671.541665914352</v>
@@ -7484,7 +7539,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v>44671.583332523151</v>
@@ -7512,7 +7567,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v>44671.624999131942</v>
@@ -7540,7 +7595,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v>44671.66666574074</v>
@@ -7568,7 +7623,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v>44671.708332349539</v>
@@ -7596,7 +7651,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v>44671.74999895833</v>
@@ -7624,7 +7679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v>44671.791665567129</v>
@@ -7652,7 +7707,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v>44671.833332175927</v>
@@ -7680,7 +7735,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v>44671.874998784719</v>
@@ -7708,7 +7763,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v>44671.916665393517</v>
@@ -7736,7 +7791,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v>44671.958332002316</v>

</xml_diff>